<commit_message>
Adicionando nova versão backlog PDF
</commit_message>
<xml_diff>
--- a/Tecnologia_da_Informação/backlog-v2.xlsx
+++ b/Tecnologia_da_Informação/backlog-v2.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivian\Documents\SPTech\Tecnologia da Informação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivian\Documents\Grupo_pi\Tecnologia_da_Informação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BB28EBF-BAB7-4E05-824F-CEF8C37FCFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1299D770-E929-4651-8C13-609206891E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{EBA81A82-E024-4BC8-9180-6AC6AA6EE44D}"/>
   </bookViews>
   <sheets>
     <sheet name="BACKLOG" sheetId="3" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BACKLOG!$A$2:$H$27</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="79">
   <si>
     <r>
       <rPr>
@@ -107,12 +110,6 @@
     <t>Desenvolver código arduíno personalizado do nosso projeto.</t>
   </si>
   <si>
-    <t>Implementar API no Sensor</t>
-  </si>
-  <si>
-    <t>Implementar API no sensor arduíno.</t>
-  </si>
-  <si>
     <t>Instalar MySQL na VMLinux</t>
   </si>
   <si>
@@ -284,10 +281,22 @@
     <t>Planejado</t>
   </si>
   <si>
-    <t>Diego Iacabo, Flávia Vaz, Heloisy Oliveira, Philipi Jordan, Samuel Sousa, Vitória Lima</t>
-  </si>
-  <si>
     <t>Grupo 2</t>
+  </si>
+  <si>
+    <t>Diego Iacabo, Flávia Vaz, Heloisy Mota, Philipi Jordan, Samuel Sousa, Vitória Lima</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>A Fazer</t>
+  </si>
+  <si>
+    <t>Em Andamento</t>
   </si>
 </sst>
 </file>
@@ -526,13 +535,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -541,11 +547,57 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -599,7 +651,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR"/>
+              <a:rPr lang="pt-BR" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Gráfico de BurnDown</a:t>
             </a:r>
           </a:p>
@@ -643,6 +702,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BACKLOG!$N$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pontos Fibonacci</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -656,24 +726,21 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>BACKLOG!$L$4:$L$7</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>Total</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Sprint1</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Sprint2</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Sprint3</c:v>
+              </c:pt>
+            </c:strLit>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -682,7 +749,78 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>270</c:v>
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0B64-4499-813E-5CD29B67E8E8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BACKLOG!$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Planejado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>Total</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Sprint1</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Sprint2</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Sprint3</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BACKLOG!$O$4:$O$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>93</c:v>
@@ -699,7 +837,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4AF1-4F3C-8004-E6FDDD72B365}"/>
+              <c16:uniqueId val="{00000001-0B64-4499-813E-5CD29B67E8E8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -712,11 +850,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="972304240"/>
-        <c:axId val="972306640"/>
+        <c:axId val="602709343"/>
+        <c:axId val="602709823"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="972304240"/>
+        <c:axId val="602709343"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -759,7 +897,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="972306640"/>
+        <c:crossAx val="602709823"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -767,7 +905,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="972306640"/>
+        <c:axId val="602709823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +956,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="972304240"/>
+        <c:crossAx val="602709343"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -830,16 +968,40 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1434,23 +1596,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>229721</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>296954</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>314884</xdr:rowOff>
+      <xdr:rowOff>363684</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>431427</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>503143</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>108858</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Gráfico 4">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E642C716-0213-94DB-3C5D-622CC3127A0E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75A8CC04-0C25-4667-D7DE-8B61AC275501}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1469,10 +1631,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1796,10 +1954,10 @@
     <tabColor theme="4" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,38 +1968,40 @@
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="I1" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="T1" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="U1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="J1" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="U1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="V1" s="18"/>
     </row>
-    <row r="2" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -1852,30 +2012,33 @@
         <v>3</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="H2" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="E3" s="8">
         <v>13</v>
@@ -1884,79 +2047,85 @@
         <v>1</v>
       </c>
       <c r="G3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" s="8">
+        <v>3</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="8">
         <f>SUMIF(G:G,1,E:E)</f>
         <v>37</v>
       </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="M3" s="16"/>
       <c r="N3" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
+        <v>33</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E4" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F4" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="8">
-        <v>2</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" s="8">
+        <v>3</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="8">
         <f>SUMIF(G:G,2,E:E)</f>
-        <v>149</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="M4" s="8">
-        <f>J6</f>
-        <v>270</v>
+        <v>141</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="N4" s="8">
-        <f>M4</f>
-        <v>270</v>
+        <f>K6</f>
+        <v>262</v>
+      </c>
+      <c r="O4" s="8">
+        <f>N4</f>
+        <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E5" s="8">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F5" s="8">
         <v>1</v>
@@ -1964,139 +2133,151 @@
       <c r="G5" s="8">
         <v>2</v>
       </c>
-      <c r="I5" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="J5" s="9">
+      <c r="H5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" s="9">
         <f>SUMIF(G:G,3,E:E)</f>
         <v>84</v>
       </c>
-      <c r="L5" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="M5" s="8">
-        <f>J3</f>
+      <c r="M5" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="8">
+        <f>K3</f>
         <v>37</v>
       </c>
-      <c r="N5" s="8">
+      <c r="O5" s="8">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>51</v>
-      </c>
       <c r="E6" s="8">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F6" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G6" s="8">
         <v>2</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" s="15">
-        <f>SUM(J3:J5)</f>
-        <v>270</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="M6" s="8">
-        <f>J4</f>
-        <v>149</v>
+      <c r="H6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" s="15">
+        <f>SUM(K3:K5)</f>
+        <v>262</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="N6" s="8">
+        <f>K4</f>
+        <v>141</v>
+      </c>
+      <c r="O6" s="8">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E7" s="8">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F7" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7" s="8">
         <v>2</v>
       </c>
-      <c r="I7" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="8">
-        <f>J6/3</f>
-        <v>90</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="M7" s="8">
-        <f>J5</f>
+      <c r="H7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" s="8">
+        <f>K6/3</f>
+        <v>87.333333333333329</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" s="8">
+        <f>K5</f>
         <v>84</v>
       </c>
-      <c r="N7" s="8">
+      <c r="O7" s="8">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
+        <v>60</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8" s="8">
         <v>13</v>
       </c>
       <c r="F8" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="8">
         <v>2</v>
       </c>
+      <c r="H8" s="8" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="9" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>6</v>
+        <v>59</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E9" s="8">
         <v>8</v>
@@ -2105,139 +2286,157 @@
         <v>1</v>
       </c>
       <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="8">
+        <v>13</v>
+      </c>
+      <c r="F10" s="8">
         <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="8">
-        <v>5</v>
-      </c>
-      <c r="F10" s="8">
-        <v>1</v>
       </c>
       <c r="G10" s="8">
         <v>1</v>
       </c>
+      <c r="H10" s="8" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="11" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="6" t="s">
+    <row r="11" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E11" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F11" s="8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G11" s="8">
         <v>2</v>
       </c>
+      <c r="H11" s="8" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="12" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="7" t="s">
+    <row r="12" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E12" s="8">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F12" s="8">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G12" s="8">
         <v>2</v>
       </c>
+      <c r="H12" s="8" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="13" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="8">
+        <v>13</v>
+      </c>
+      <c r="F13" s="8">
+        <v>2</v>
+      </c>
+      <c r="G13" s="8">
+        <v>2</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="8">
-        <v>5</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1</v>
-      </c>
-      <c r="G13" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E14" s="8">
         <v>8</v>
       </c>
       <c r="F14" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G14" s="8">
         <v>2</v>
       </c>
+      <c r="H14" s="8" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="15" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E15" s="8">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F15" s="8">
         <v>1</v>
@@ -2245,275 +2444,311 @@
       <c r="G15" s="8">
         <v>2</v>
       </c>
+      <c r="H15" s="8" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="16" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>21</v>
+        <v>55</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E16" s="8">
+        <v>5</v>
+      </c>
+      <c r="F16" s="8">
+        <v>3</v>
+      </c>
+      <c r="G16" s="8">
+        <v>1</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="8">
+        <v>8</v>
+      </c>
+      <c r="F17" s="8">
+        <v>8</v>
+      </c>
+      <c r="G17" s="8">
+        <v>2</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="8">
         <v>13</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F18" s="8">
+        <v>5</v>
+      </c>
+      <c r="G18" s="8">
         <v>2</v>
       </c>
-      <c r="G16" s="8">
-        <v>3</v>
+      <c r="H18" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="8">
-        <v>13</v>
-      </c>
-      <c r="F17" s="8">
-        <v>2</v>
-      </c>
-      <c r="G17" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="8">
-        <v>3</v>
-      </c>
-      <c r="F18" s="8">
-        <v>2</v>
-      </c>
-      <c r="G18" s="8">
+    <row r="19" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="8">
+        <v>5</v>
+      </c>
+      <c r="F19" s="8">
         <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="8">
-        <v>3</v>
-      </c>
-      <c r="F19" s="8">
-        <v>2</v>
       </c>
       <c r="G19" s="8">
         <v>1</v>
       </c>
+      <c r="H19" s="8" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="20" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="8">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F20" s="8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G20" s="8">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E21" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F21" s="8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G21" s="8">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E22" s="8">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F22" s="8">
         <v>1</v>
       </c>
       <c r="G22" s="8">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E23" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F23" s="8">
+        <v>2</v>
+      </c>
+      <c r="G23" s="8">
+        <v>3</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="8">
+        <v>3</v>
+      </c>
+      <c r="F24" s="8">
+        <v>2</v>
+      </c>
+      <c r="G24" s="8">
         <v>1</v>
       </c>
-      <c r="G23" s="8">
-        <v>2</v>
+      <c r="H24" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="8">
-        <v>13</v>
-      </c>
-      <c r="F24" s="8">
+    <row r="25" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="8">
+        <v>3</v>
+      </c>
+      <c r="F25" s="8">
         <v>1</v>
       </c>
-      <c r="G24" s="8">
-        <v>2</v>
+      <c r="G25" s="8">
+        <v>1</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="6" t="s">
+    <row r="26" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="8">
         <v>21</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="8">
-        <v>13</v>
-      </c>
-      <c r="F25" s="8">
-        <v>2</v>
-      </c>
-      <c r="G25" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" s="8">
-        <v>8</v>
       </c>
       <c r="F26" s="8">
         <v>2</v>
       </c>
       <c r="G26" s="8">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E27" s="8">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F27" s="8">
         <v>1</v>
@@ -2521,36 +2756,28 @@
       <c r="G27" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="8">
-        <v>8</v>
-      </c>
-      <c r="F28" s="8">
-        <v>1</v>
-      </c>
-      <c r="G28" s="8">
-        <v>3</v>
+      <c r="H27" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:H27" xr:uid="{74A2642B-D400-46EA-964E-E05A5AEA6485}"/>
   <mergeCells count="3">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="I1:R1"/>
-    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="J1:S1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Em Andamento">
+      <formula>NOT(ISERROR(SEARCH("Em Andamento",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Concluído">
+      <formula>NOT(ISERROR(SEARCH("Concluído",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="A Fazer">
+      <formula>NOT(ISERROR(SEARCH("A Fazer",H1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="7" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2558,14 +2785,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2574,7 +2793,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A729CFA7192B0F4AA60BE2DF65F4BC74" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee39750ad8b983f0f9ac05c6d33cdc04">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="575218e2c9ab049ab6ad7cca76d1d38a" ns3:_="">
     <xsd:import namespace="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
@@ -2768,23 +2987,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44DAEA0-DD6E-45E5-938F-CB046081399A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAE2E3D6-6D5D-436A-9712-0442BFABA7F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2792,7 +3003,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90D062E9-275A-40A9-8059-A8AD790EE81A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2808,4 +3019,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44DAEA0-DD6E-45E5-938F-CB046081399A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Atualização do backlog após a sprint review
</commit_message>
<xml_diff>
--- a/Tecnologia_da_Informação/backlog-v2.xlsx
+++ b/Tecnologia_da_Informação/backlog-v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2d5518b78ed5f75/Documentos/grupo_pi/Grupo_pi/Tecnologia_da_Informação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{1299D770-E929-4651-8C13-609206891E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADCACD5D-F8BD-4670-B1AD-730C80EA9F0C}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="8_{1299D770-E929-4651-8C13-609206891E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D9B2166-C4CC-427E-B111-DCDB89F61739}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EBA81A82-E024-4BC8-9180-6AC6AA6EE44D}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="BACKLOG" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BACKLOG!$A$2:$H$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BACKLOG!$A$2:$H$35</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="96">
   <si>
     <r>
       <rPr>
@@ -173,18 +173,6 @@
     <t>Criação de Gráficos com ChartJS</t>
   </si>
   <si>
-    <t>Definir métricas e indicadores do Dashboard</t>
-  </si>
-  <si>
-    <t>Criar os gráficos da Dashboard usando a API ChartJS para melhor visualização dos dados.</t>
-  </si>
-  <si>
-    <t>Conectar a API com o Banco de Dados para que os dados captados pelo sensor possam ser armazenados nas tabelas.</t>
-  </si>
-  <si>
-    <t>Definir as medidas (quantitativas ou qualitativas) que serão disponibilizadas na Dashboard.</t>
-  </si>
-  <si>
     <t>Tamanho</t>
   </si>
   <si>
@@ -221,12 +209,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>Criar aba para criação de conta das seguradoras.</t>
-  </si>
-  <si>
-    <t>Aba para as seguradoras acessarem o site.</t>
-  </si>
-  <si>
     <t>Instalar máquina virtual Lubuntu.</t>
   </si>
   <si>
@@ -297,6 +279,75 @@
   </si>
   <si>
     <t>Concluido</t>
+  </si>
+  <si>
+    <t>Criar usuário para exibir consultas</t>
+  </si>
+  <si>
+    <t>Criar usuário para inserir dados</t>
+  </si>
+  <si>
+    <t>Criar o usuário (dat_acq_ino) no banco de dados para a API dat_acqu_ino da máquina virtual para inserir dados nas tabelas, garantindo a segurança do sistema.</t>
+  </si>
+  <si>
+    <t>Criar o usuário (web_data_viz) no banco de dados da máquina virtual para realizar consultas, garantindo a segurança do sistema.</t>
+  </si>
+  <si>
+    <t>Integrar a API do Google Maps</t>
+  </si>
+  <si>
+    <t>Integrar a API do Google Maps na dashboard da Zona Azul e das Seguradoras.</t>
+  </si>
+  <si>
+    <t>Criar dashboard do parceiro Zona Azul</t>
+  </si>
+  <si>
+    <t>Criar dashboard para o nosso parceiro Zona Azul, com o objetivo de tornar mais visual a situação da ocupação das vagas.</t>
+  </si>
+  <si>
+    <t>Em Andamento</t>
+  </si>
+  <si>
+    <t>Implementar ferramenta de Help Desk</t>
+  </si>
+  <si>
+    <t>Implementar a ferramenta de Help Desk Jira no fluxo de produções do projeto.</t>
+  </si>
+  <si>
+    <t>Criar fluxo de suporte ao cliente</t>
+  </si>
+  <si>
+    <t>Criar um fluxograma do suporte ao cliente, contendo as principais etapas do processo de atendimento ao cliente.</t>
+  </si>
+  <si>
+    <t>Implementar  BobIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar a Inteligência Artificial Bob no fluxo de suporte ao cliente. </t>
+  </si>
+  <si>
+    <t>Criar SLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar o acordo formal que define os níveis de serviço. </t>
+  </si>
+  <si>
+    <t>Criar aba estática para criação de conta das seguradoras.</t>
+  </si>
+  <si>
+    <t>Criar Aba estática para as seguradoras acessarem o site.</t>
+  </si>
+  <si>
+    <t>Conectar a API dat_acqu_ino com o Banco de Dados para que os dados captados pelo sensor possam ser armazenados nas tabelas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definir métricas e indicadores da Dashboard das seguradoras </t>
+  </si>
+  <si>
+    <t>Definir as medidas (quantitativas ou qualitativas) que serão disponibilizadas na Dashboard das seguradoras.</t>
+  </si>
+  <si>
+    <t>Criar os gráficos da Dashboard das seguradoras usando a API ChartJS para melhor visualização dos dados, além de adicionar as KPIs relevantes para o cliente.</t>
   </si>
 </sst>
 </file>
@@ -497,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -547,6 +598,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -554,12 +608,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -707,7 +755,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="FFC60D"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -740,7 +788,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>262</c:v>
+                  <c:v>361</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>37</c:v>
@@ -749,7 +797,7 @@
                   <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -778,7 +826,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -811,7 +859,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>262</c:v>
+                  <c:v>361</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>93</c:v>
@@ -820,7 +868,7 @@
                   <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1945,10 +1993,10 @@
     <tabColor theme="4" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V27"/>
+  <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="131" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1965,32 +2013,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="J1" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="U1" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="V1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="J1" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="U1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="V1" s="19"/>
     </row>
     <row r="2" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
@@ -2003,19 +2051,19 @@
         <v>3</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2023,28 +2071,28 @@
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E3" s="8">
         <v>13</v>
       </c>
       <c r="F3" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G3" s="8">
         <v>3</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="K3" s="8">
         <f>SUMIF(G:G,1,E:E)</f>
@@ -2052,10 +2100,10 @@
       </c>
       <c r="M3" s="16"/>
       <c r="N3" s="14" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2069,37 +2117,37 @@
         <v>19</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E4" s="8">
         <v>13</v>
       </c>
       <c r="F4" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G4" s="8">
         <v>3</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="K4" s="8">
         <f>SUMIF(G:G,2,E:E)</f>
         <v>141</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="N4" s="8">
         <f>K6</f>
-        <v>262</v>
+        <v>361</v>
       </c>
       <c r="O4" s="8">
         <f>N4</f>
-        <v>262</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2113,7 +2161,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E5" s="8">
         <v>13</v>
@@ -2124,18 +2172,18 @@
       <c r="G5" s="8">
         <v>2</v>
       </c>
-      <c r="H5" s="21" t="s">
-        <v>78</v>
+      <c r="H5" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="K5" s="9">
         <f>SUMIF(G:G,3,E:E)</f>
-        <v>84</v>
+        <v>183</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="N5" s="8">
         <f>K3</f>
@@ -2150,13 +2198,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E6" s="8">
         <v>5</v>
@@ -2168,17 +2216,17 @@
         <v>2</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="K6" s="15">
         <f>SUM(K3:K5)</f>
-        <v>262</v>
+        <v>361</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="N6" s="8">
         <f>K4</f>
@@ -2193,13 +2241,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E7" s="8">
         <v>8</v>
@@ -2211,38 +2259,38 @@
         <v>2</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="K7" s="8">
         <f>K6/3</f>
-        <v>87.333333333333329</v>
+        <v>120.33333333333333</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="N7" s="8">
         <f>K5</f>
-        <v>84</v>
+        <v>183</v>
       </c>
       <c r="O7" s="8">
-        <v>84</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E8" s="8">
         <v>13</v>
@@ -2253,22 +2301,22 @@
       <c r="G8" s="8">
         <v>2</v>
       </c>
-      <c r="H8" s="21" t="s">
-        <v>78</v>
+      <c r="H8" s="17" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E9" s="8">
         <v>8</v>
@@ -2279,8 +2327,8 @@
       <c r="G9" s="8">
         <v>1</v>
       </c>
-      <c r="H9" s="21" t="s">
-        <v>78</v>
+      <c r="H9" s="17" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2294,7 +2342,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E10" s="8">
         <v>13</v>
@@ -2306,7 +2354,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2314,13 +2362,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E11" s="8">
         <v>8</v>
@@ -2332,7 +2380,7 @@
         <v>2</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2346,7 +2394,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E12" s="8">
         <v>21</v>
@@ -2358,7 +2406,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2366,13 +2414,13 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E13" s="8">
         <v>13</v>
@@ -2384,7 +2432,7 @@
         <v>2</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2392,13 +2440,13 @@
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E14" s="8">
         <v>8</v>
@@ -2410,7 +2458,7 @@
         <v>2</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2424,7 +2472,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E15" s="8">
         <v>5</v>
@@ -2435,22 +2483,22 @@
       <c r="G15" s="8">
         <v>2</v>
       </c>
-      <c r="H15" s="20" t="s">
-        <v>78</v>
+      <c r="H15" s="17" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E16" s="8">
         <v>5</v>
@@ -2461,8 +2509,8 @@
       <c r="G16" s="8">
         <v>1</v>
       </c>
-      <c r="H16" s="21" t="s">
-        <v>78</v>
+      <c r="H16" s="17" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2476,7 +2524,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E17" s="8">
         <v>8</v>
@@ -2487,8 +2535,8 @@
       <c r="G17" s="8">
         <v>2</v>
       </c>
-      <c r="H17" s="21" t="s">
-        <v>78</v>
+      <c r="H17" s="17" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2496,13 +2544,13 @@
         <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E18" s="8">
         <v>13</v>
@@ -2514,7 +2562,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2528,7 +2576,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E19" s="8">
         <v>5</v>
@@ -2539,22 +2587,22 @@
       <c r="G19" s="8">
         <v>1</v>
       </c>
-      <c r="H19" s="21" t="s">
-        <v>78</v>
+      <c r="H19" s="17" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>37</v>
+      <c r="A20" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E20" s="8">
         <v>13</v>
@@ -2566,7 +2614,7 @@
         <v>2</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2574,13 +2622,13 @@
         <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E21" s="8">
         <v>13</v>
@@ -2592,21 +2640,21 @@
         <v>2</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E22" s="8">
         <v>21</v>
@@ -2618,21 +2666,21 @@
         <v>3</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E23" s="8">
         <v>8</v>
@@ -2644,7 +2692,7 @@
         <v>3</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2658,7 +2706,7 @@
         <v>22</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E24" s="8">
         <v>3</v>
@@ -2670,7 +2718,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2684,7 +2732,7 @@
         <v>22</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E25" s="8">
         <v>3</v>
@@ -2696,7 +2744,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2710,19 +2758,19 @@
         <v>22</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E26" s="8">
         <v>21</v>
       </c>
       <c r="F26" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G26" s="8">
         <v>3</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2736,23 +2784,231 @@
         <v>22</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E27" s="8">
         <v>8</v>
       </c>
       <c r="F27" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G27" s="8">
         <v>3</v>
       </c>
       <c r="H27" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="8">
+        <v>5</v>
+      </c>
+      <c r="F28" s="8">
+        <v>2</v>
+      </c>
+      <c r="G28" s="8">
+        <v>3</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="8">
+        <v>5</v>
+      </c>
+      <c r="F29" s="8">
+        <v>1</v>
+      </c>
+      <c r="G29" s="8">
+        <v>3</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="B30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="8">
+        <v>21</v>
+      </c>
+      <c r="F30" s="8">
+        <v>2</v>
+      </c>
+      <c r="G30" s="8">
+        <v>3</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="8">
+        <v>13</v>
+      </c>
+      <c r="F31" s="8">
+        <v>1</v>
+      </c>
+      <c r="G31" s="8">
+        <v>3</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="8">
+        <v>13</v>
+      </c>
+      <c r="F32" s="8">
+        <v>4</v>
+      </c>
+      <c r="G32" s="8">
+        <v>3</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="8">
+        <v>13</v>
+      </c>
+      <c r="F33" s="8">
+        <v>3</v>
+      </c>
+      <c r="G33" s="8">
+        <v>3</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="8">
+        <v>21</v>
+      </c>
+      <c r="F34" s="8">
+        <v>6</v>
+      </c>
+      <c r="G34" s="8">
+        <v>3</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="8">
+        <v>8</v>
+      </c>
+      <c r="F35" s="8">
+        <v>3</v>
+      </c>
+      <c r="G35" s="8">
+        <v>3</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H27" xr:uid="{74A2642B-D400-46EA-964E-E05A5AEA6485}"/>
+  <autoFilter ref="A2:H35" xr:uid="{74A2642B-D400-46EA-964E-E05A5AEA6485}"/>
   <mergeCells count="3">
     <mergeCell ref="J1:S1"/>
     <mergeCell ref="U1:V1"/>
@@ -2776,6 +3032,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A729CFA7192B0F4AA60BE2DF65F4BC74" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee39750ad8b983f0f9ac05c6d33cdc04">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="575218e2c9ab049ab6ad7cca76d1d38a" ns3:_="">
     <xsd:import namespace="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
@@ -2969,14 +3233,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2987,6 +3243,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44DAEA0-DD6E-45E5-938F-CB046081399A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90D062E9-275A-40A9-8059-A8AD790EE81A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3004,22 +3276,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44DAEA0-DD6E-45E5-938F-CB046081399A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAE2E3D6-6D5D-436A-9712-0442BFABA7F1}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Alteração no script de banco de dados
</commit_message>
<xml_diff>
--- a/Tecnologia_da_Informação/backlog-v2.xlsx
+++ b/Tecnologia_da_Informação/backlog-v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2d5518b78ed5f75/Documentos/grupo_pi/Grupo_pi/Tecnologia_da_Informação/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b951b5393c7c3979/Documentos/grupo_pi/Grupo_pi/Tecnologia_da_Informação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{1299D770-E929-4651-8C13-609206891E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D9B2166-C4CC-427E-B111-DCDB89F61739}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="8_{1299D770-E929-4651-8C13-609206891E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3309597-923A-442D-BA90-B5EF350B6F94}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EBA81A82-E024-4BC8-9180-6AC6AA6EE44D}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{EBA81A82-E024-4BC8-9180-6AC6AA6EE44D}"/>
   </bookViews>
   <sheets>
     <sheet name="BACKLOG" sheetId="3" r:id="rId1"/>
@@ -1672,6 +1672,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -1995,8 +1999,8 @@
   </sheetPr>
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="131" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="H7" zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3032,14 +3036,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A729CFA7192B0F4AA60BE2DF65F4BC74" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee39750ad8b983f0f9ac05c6d33cdc04">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="575218e2c9ab049ab6ad7cca76d1d38a" ns3:_="">
     <xsd:import namespace="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
@@ -3233,7 +3229,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3242,23 +3238,15 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44DAEA0-DD6E-45E5-938F-CB046081399A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90D062E9-275A-40A9-8059-A8AD790EE81A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3276,10 +3264,26 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAE2E3D6-6D5D-436A-9712-0442BFABA7F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44DAEA0-DD6E-45E5-938F-CB046081399A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>